<commit_message>
#ES-272 - updated experiments-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-server/src/main/resources/report-templates/experiments-report-template.xlsx
+++ b/eca-server/src/main/resources/report-templates/experiments-report-template.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -156,9 +157,6 @@
     <t>Метод оценки точности</t>
   </si>
   <si>
-    <t>Email заявки</t>
-  </si>
-  <si>
     <t>Обучающая выборка</t>
   </si>
   <si>
@@ -192,9 +190,6 @@
     <t>${experiment.evaluationMethod}</t>
   </si>
   <si>
-    <t>${experiment.email}</t>
-  </si>
-  <si>
     <t>${experiment.evaluationTotalTime}</t>
   </si>
   <si>
@@ -217,6 +212,12 @@
   </si>
   <si>
     <t>${experiment.experimentPath}</t>
+  </si>
+  <si>
+    <t>Пользователь</t>
+  </si>
+  <si>
+    <t>${experiment.createdBy}</t>
   </si>
 </sst>
 </file>
@@ -733,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:L8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -848,71 +849,71 @@
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>

</xml_diff>

<commit_message>
#ES-282 - added Experiment#maxPctCorrect column
</commit_message>
<xml_diff>
--- a/eca-server/src/main/resources/report-templates/experiments-report-template.xlsx
+++ b/eca-server/src/main/resources/report-templates/experiments-report-template.xlsx
@@ -38,7 +38,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:area(lastCell="L8")</t>
+          <t>jx:area(lastCell="M8")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="L3", areas=["A3:B3"])</t>
+          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="M3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -88,7 +88,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.filters" var="filter" lastCell="L4")</t>
+          <t>jx:each(items="report.filters" var="filter" lastCell="M4")</t>
         </r>
       </text>
     </comment>
@@ -113,7 +113,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.items" var="experiment" lastCell="L7")</t>
+          <t>jx:each(items="report.items" var="experiment" lastCell="M7")</t>
         </r>
       </text>
     </comment>
@@ -148,15 +148,34 @@
     <t>Статус заявки</t>
   </si>
   <si>
-    <t>Метод оценки точности</t>
-  </si>
-  <si>
-    <t>Пользователь</t>
+    <t>Точность наилучшего классификатора, %</t>
   </si>
   <si>
     <t>Обучающая выборка</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Метод оценки точности</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>Пользователь</t>
+    </r>
+  </si>
+  <si>
     <t>Модель эксперимента</t>
   </si>
   <si>
@@ -184,13 +203,44 @@
     <t>${experiment.requestStatus}</t>
   </si>
   <si>
-    <t>${experiment.evaluationMethod}</t>
-  </si>
-  <si>
-    <t>${experiment.createdBy}</t>
-  </si>
-  <si>
-    <t>${experiment.relationName}</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${experiment.maxPctCorrect}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${experiment.relationName}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${experiment.evaluationMethod}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${experiment.createdBy}</t>
+    </r>
   </si>
   <si>
     <t>${experiment.modelPath}</t>
@@ -321,20 +371,12 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="1000" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="1000" quotePrefix="false"/>
-    <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
-    <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="3" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="3" fontId="0" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="2" numFmtId="1000" quotePrefix="false"/>
-    <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="0" numFmtId="1000" quotePrefix="false">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="0" numFmtId="1000" quotePrefix="false">
-      <alignment wrapText="true"/>
-    </xf>
     <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="0" numFmtId="1000" quotePrefix="false">
       <alignment wrapText="true"/>
     </xf>
@@ -571,7 +613,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:AMI8"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -580,196 +622,209 @@
     <col customWidth="true" max="1" min="1" outlineLevel="0" width="43.6640623533012"/>
     <col customWidth="true" max="2" min="2" outlineLevel="0" width="40.2187508193987"/>
     <col customWidth="true" max="3" min="3" outlineLevel="0" width="28.8867197273312"/>
-    <col customWidth="true" max="4" min="4" outlineLevel="0" width="36.554687112768"/>
-    <col customWidth="true" max="5" min="5" outlineLevel="0" width="31.0000005074985"/>
-    <col customWidth="true" max="6" min="6" outlineLevel="0" width="51.8867161748414"/>
-    <col customWidth="true" max="7" min="7" outlineLevel="0" width="59.5546862669371"/>
-    <col customWidth="true" max="8" min="8" outlineLevel="0" width="37.8867178665032"/>
-    <col customWidth="true" max="9" min="9" outlineLevel="0" width="26.9999998308338"/>
-    <col customWidth="true" max="10" min="10" outlineLevel="0" width="30.8867187123341"/>
-    <col customWidth="true" max="11" min="11" outlineLevel="0" width="34.3320302462366"/>
-    <col customWidth="true" max="12" min="12" outlineLevel="0" width="31.5546869436019"/>
-    <col customWidth="true" max="1023" min="13" outlineLevel="0" width="8.55468778943276"/>
+    <col customWidth="true" hidden="false" max="4" min="4" outlineLevel="0" width="40.1706183040853"/>
+    <col customWidth="true" max="5" min="5" outlineLevel="0" width="36.554687112768"/>
+    <col customWidth="true" max="6" min="6" outlineLevel="0" width="31.0000005074985"/>
+    <col customWidth="true" max="7" min="7" outlineLevel="0" width="51.8867161748414"/>
+    <col customWidth="true" max="8" min="8" outlineLevel="0" width="59.5546862669371"/>
+    <col customWidth="true" max="9" min="9" outlineLevel="0" width="37.8867178665032"/>
+    <col customWidth="true" max="10" min="10" outlineLevel="0" width="26.9999998308338"/>
+    <col customWidth="true" max="11" min="11" outlineLevel="0" width="30.8867187123341"/>
+    <col customWidth="true" max="12" min="12" outlineLevel="0" width="34.3320302462366"/>
+    <col customWidth="true" max="13" min="13" outlineLevel="0" width="31.5546869436019"/>
+    <col customWidth="true" max="1024" min="14" outlineLevel="0" width="8.55468778943276"/>
   </cols>
   <sheetData>
     <row ht="15.6000003814697" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s"/>
-      <c r="C1" s="2" t="s"/>
-      <c r="D1" s="2" t="s"/>
-      <c r="E1" s="2" t="s"/>
-      <c r="F1" s="2" t="s"/>
-      <c r="G1" s="2" t="s"/>
-      <c r="H1" s="2" t="s"/>
-      <c r="I1" s="2" t="s"/>
-      <c r="J1" s="2" t="s"/>
-      <c r="K1" s="2" t="s"/>
-      <c r="L1" s="3" t="s"/>
+      <c r="B1" s="1" t="s"/>
+      <c r="C1" s="1" t="s"/>
+      <c r="D1" s="1" t="s"/>
+      <c r="E1" s="1" t="s"/>
+      <c r="F1" s="1" t="s"/>
+      <c r="G1" s="1" t="s"/>
+      <c r="H1" s="1" t="s"/>
+      <c r="I1" s="1" t="s"/>
+      <c r="J1" s="1" t="s"/>
+      <c r="K1" s="1" t="s"/>
+      <c r="L1" s="1" t="s"/>
+      <c r="M1" s="1" t="s"/>
     </row>
     <row ht="15.6000003814697" outlineLevel="0" r="2">
-      <c r="A2" s="4" t="n"/>
-      <c r="B2" s="5" t="n"/>
-      <c r="C2" s="5" t="n"/>
-      <c r="D2" s="5" t="n"/>
-      <c r="E2" s="5" t="n"/>
-      <c r="F2" s="5" t="n"/>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="5" t="n"/>
-      <c r="I2" s="5" t="n"/>
-      <c r="J2" s="5" t="n"/>
-      <c r="K2" s="5" t="n"/>
-      <c r="L2" s="5" t="n"/>
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="n"/>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+      <c r="M2" s="3" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s"/>
-      <c r="D3" s="8" t="s"/>
-      <c r="E3" s="8" t="s"/>
-      <c r="F3" s="8" t="s"/>
-      <c r="G3" s="8" t="s"/>
-      <c r="H3" s="8" t="s"/>
-      <c r="I3" s="8" t="s"/>
-      <c r="J3" s="8" t="s"/>
-      <c r="K3" s="8" t="s"/>
-      <c r="L3" s="9" t="s"/>
+      <c r="C3" s="5" t="s"/>
+      <c r="D3" s="5" t="s"/>
+      <c r="E3" s="5" t="s"/>
+      <c r="F3" s="5" t="s"/>
+      <c r="G3" s="5" t="s"/>
+      <c r="H3" s="5" t="s"/>
+      <c r="I3" s="5" t="s"/>
+      <c r="J3" s="5" t="s"/>
+      <c r="K3" s="5" t="s"/>
+      <c r="L3" s="5" t="s"/>
+      <c r="M3" s="5" t="s"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s"/>
-      <c r="D4" s="8" t="s"/>
-      <c r="E4" s="8" t="s"/>
-      <c r="F4" s="8" t="s"/>
-      <c r="G4" s="8" t="s"/>
-      <c r="H4" s="8" t="s"/>
-      <c r="I4" s="8" t="s"/>
-      <c r="J4" s="8" t="s"/>
-      <c r="K4" s="8" t="s"/>
-      <c r="L4" s="9" t="s"/>
+      <c r="C4" s="5" t="s"/>
+      <c r="D4" s="5" t="s"/>
+      <c r="E4" s="5" t="s"/>
+      <c r="F4" s="5" t="s"/>
+      <c r="G4" s="5" t="s"/>
+      <c r="H4" s="5" t="s"/>
+      <c r="I4" s="5" t="s"/>
+      <c r="J4" s="5" t="s"/>
+      <c r="K4" s="5" t="s"/>
+      <c r="L4" s="5" t="s"/>
+      <c r="M4" s="5" t="s"/>
     </row>
     <row outlineLevel="0" r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="5" t="n"/>
-      <c r="C5" s="5" t="n"/>
-      <c r="D5" s="5" t="n"/>
-      <c r="E5" s="5" t="n"/>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="5" t="n"/>
-      <c r="H5" s="5" t="n"/>
-      <c r="I5" s="5" t="n"/>
-      <c r="J5" s="5" t="n"/>
-      <c r="K5" s="5" t="n"/>
-      <c r="L5" s="5" t="n"/>
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+      <c r="M5" s="3" t="n"/>
     </row>
     <row outlineLevel="0" r="6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="7" t="s">
         <v>16</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row outlineLevel="0" r="7">
-      <c r="A7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="H7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="J7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="K7" s="9" t="s">
         <v>28</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row outlineLevel="0" r="8">
-      <c r="A8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="15" t="s"/>
-      <c r="C8" s="15" t="s"/>
-      <c r="D8" s="15" t="s"/>
-      <c r="E8" s="15" t="s"/>
-      <c r="F8" s="15" t="s"/>
-      <c r="G8" s="15" t="s"/>
-      <c r="H8" s="15" t="s"/>
-      <c r="I8" s="15" t="s"/>
-      <c r="J8" s="15" t="s"/>
-      <c r="K8" s="15" t="s"/>
-      <c r="L8" s="16" t="s"/>
+      <c r="A8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s"/>
+      <c r="C8" s="11" t="s"/>
+      <c r="D8" s="11" t="s"/>
+      <c r="E8" s="11" t="s"/>
+      <c r="F8" s="11" t="s"/>
+      <c r="G8" s="11" t="s"/>
+      <c r="H8" s="11" t="s"/>
+      <c r="I8" s="11" t="s"/>
+      <c r="J8" s="11" t="s"/>
+      <c r="K8" s="11" t="s"/>
+      <c r="L8" s="11" t="s"/>
+      <c r="M8" s="12" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="A8:M8"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.511805534362793" header="0.511805534362793" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
   <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297mm" paperSize="9" paperWidth="210mm" scale="100"/>

</xml_diff>